<commit_message>
Atualiza dicionario de orgaos (formatos 'XLSX' e 'RData')
</commit_message>
<xml_diff>
--- a/R/rDOU/inst/extdata/des_orgao.xlsx
+++ b/R/rDOU/inst/extdata/des_orgao.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>GABINETE DO MINISTRO</t>
   </si>
@@ -219,9 +219,6 @@
     <t>SFA-TO/MAPA</t>
   </si>
   <si>
-    <t>SUPERINTENDÊNCIA FEDERAL DO DISTRITO FEDERAL</t>
-  </si>
-  <si>
     <t>SFA-DF/MAPA</t>
   </si>
   <si>
@@ -229,6 +226,45 @@
   </si>
   <si>
     <t>DES_ORGAO</t>
+  </si>
+  <si>
+    <t>SUPERINTENDÊNCIA FEDERAL NO DISTRITO FEDERAL</t>
+  </si>
+  <si>
+    <t>SECRETARIA DE MOBILIDADE SOCIAL, DO PRODUTOR RURAL E DO COOPERATIVISMO</t>
+  </si>
+  <si>
+    <t>COMISSÃO EXECUTIVA DO PLANO DA LAVOURA CACAUEIRA</t>
+  </si>
+  <si>
+    <t>CEPLAC/MAPA</t>
+  </si>
+  <si>
+    <t>EMPRESA BRASILEIRA DE PESQUISA AGROPECUÁRIA</t>
+  </si>
+  <si>
+    <t>EMBRAPA/MAPA</t>
+  </si>
+  <si>
+    <t>SECRETARIA DE INTEGRAÇÃO E MOBILIDADE SOCIAL</t>
+  </si>
+  <si>
+    <t>SECRETARIA DO PRODUTOR RURAL E COOPERATIVISMO</t>
+  </si>
+  <si>
+    <t>SECRETARIA DE AQUICULTURA E PESCA</t>
+  </si>
+  <si>
+    <t>SECRETARIA DE PRODUÇÃO E AGROENERGIA</t>
+  </si>
+  <si>
+    <t>SPAE/MAPA</t>
+  </si>
+  <si>
+    <t>SDC/MAPA</t>
+  </si>
+  <si>
+    <t>SECRETARIA DE DESENVOLVIMENTO AGROPECUÁRIO E COOPERATIVISMO</t>
   </si>
 </sst>
 </file>
@@ -562,24 +598,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="103.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
         <v>67</v>
-      </c>
-      <c r="B1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -629,225 +665,277 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>43</v>
-      </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>44</v>
-      </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>64</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B43" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Teste completo de acordo com o gabarito. Todos os testes passando.
</commit_message>
<xml_diff>
--- a/R/rDOU/inst/extdata/des_orgao.xlsx
+++ b/R/rDOU/inst/extdata/des_orgao.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas.barcellos\Desktop\Projetos\Controle\projdiario\R\rDOU\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas.barcellos\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="8670"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>GABINETE DO MINISTRO</t>
   </si>
@@ -265,6 +265,18 @@
   </si>
   <si>
     <t>SECRETARIA DE DESENVOLVIMENTO AGROPECUÁRIO E COOPERATIVISMO</t>
+  </si>
+  <si>
+    <t>SAP/MAPA</t>
+  </si>
+  <si>
+    <t>SPRC/MAPA</t>
+  </si>
+  <si>
+    <t>SMC/MAPA</t>
+  </si>
+  <si>
+    <t>SIMS/MAPA</t>
   </si>
 </sst>
 </file>
@@ -601,7 +613,7 @@
   <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,6 +692,9 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
       <c r="B10" t="s">
         <v>69</v>
       </c>
@@ -701,16 +716,25 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
       <c r="B13" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
       <c r="B14" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
       <c r="B15" t="s">
         <v>75</v>
       </c>

</xml_diff>